<commit_message>
Atualização automática de SAPUCAIA_DO_SUL.xlsx
</commit_message>
<xml_diff>
--- a/SAPUCAIA_DO_SUL.xlsx
+++ b/SAPUCAIA_DO_SUL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95E0467C-DBC8-4DD8-A123-FD866E4A8257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C15B0B2D-66F9-42CD-B7AE-E53BA39A149E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1218,7 +1218,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{2A4FB8C2-204F-49B5-A786-2DB06B2E051C}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{8E604A0E-740A-4370-ACA1-B22959B1B428}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1248,10 +1248,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBE39849-4687-4B01-A166-84EE55F28AC6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C6CED2E-53E9-472F-A675-102C5A09E65B}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1289,7 +1289,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ADDC15C-3481-4A1C-A547-0BD35867E17B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D8DF8C6-0DDC-4653-AF8B-5F64FE9326B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1352,7 +1352,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B431471A-38D7-4EAD-8ACA-5B79E4872610}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7F4960-4D45-418C-871B-A4D3B1897779}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1371,7 +1371,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6E34584-E01A-A9A3-7C14-99B6019C1666}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0799FE58-AA11-1D35-7FB9-10ABB8E838D7}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1420,7 +1420,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B026063-F4CA-A8DF-D2DF-256D236D25B5}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98D554A3-7CDF-29AB-2E27-50DE37377C65}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1439,7 +1439,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EEF70A3-CE9E-ABD3-D1C2-496114A117B4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1563313-B485-10CC-F71F-DF8F28A221AE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1470,7 +1470,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23345E9B-9011-A38E-73C5-5438FEE44ED3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C91977B8-3BDE-1A86-A24F-544E6A562285}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1501,7 +1501,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B32090A5-6A01-D255-B70F-2A83D96BE150}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50D917FF-CF74-294C-F7FF-D6BD1DF9CB1F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1544,7 +1544,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45810781-B776-444A-B687-DBD8254BE941}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD65F677-67E3-4387-9143-30C4A4013A61}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1582,7 +1582,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F00EA0DA-1CF7-4C6E-B1C6-8AE577485981}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08F6AC47-F3AB-48C4-A85C-B2607939842F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1625,7 +1625,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0409D160-2F98-4ACD-94C9-D1E7C2195E2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8449BDA-6072-4D9D-B301-D71E8D89C693}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1938,7 +1938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8790F25B-4974-4741-8A08-922F6F013583}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7609E0EB-3BBE-497B-8A53-C6125618CCED}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>